<commit_message>
Simple Working Expense Tracker v1
</commit_message>
<xml_diff>
--- a/PersonalExpenseTracker/Documentation/Expense Tracker.xlsx
+++ b/PersonalExpenseTracker/Documentation/Expense Tracker.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Projects\PythonProjects\PersonalExpenseTracker\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D53FC0A-4FD6-4DAD-BAFB-0BA7DCE741A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Category</t>
   </si>
@@ -158,55 +167,185 @@
   </si>
   <si>
     <t>For storing data in a relational database.</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Category Storage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Store categories in a separate CSV file (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>categories.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Add Category</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allow the user to add new categories, which will be saved to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>categories.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>List Categories</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Read and display categories from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>categories.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Choose Category</t>
+  </si>
+  <si>
+    <t>When adding an expense, prompt the user to choose a category from the list.</t>
+  </si>
+  <si>
+    <t>Expense Storage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Save expenses (including category) in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>expenses.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
-    <border/>
+  <borders count="6">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -218,6 +357,10 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -226,6 +369,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -234,49 +382,87 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -466,25 +652,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.5"/>
-    <col customWidth="1" min="2" max="2" width="31.63"/>
-    <col customWidth="1" min="3" max="3" width="59.63"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,202 +686,250 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="4"/>
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="36" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="42" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="36.75" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="39.75" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A20"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>